<commit_message>
Atualização Base de dados Emails
</commit_message>
<xml_diff>
--- a/Bases de Dados/Emails.xlsx
+++ b/Bases de Dados/Emails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Python Impressionador\Projeto_AutomacaoIndicadores\Bases de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\Projetos Hashtag\Projeto1 - Automação de Processo\Projeto\Bases de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3856DD-4A41-42A6-8CEE-9B800498E7C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFE9307-ECFA-4BA7-BEF0-C53ABB8933CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{EE9D8D8A-F7B1-481B-B9DF-10FF6CFE8B3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EE9D8D8A-F7B1-481B-B9DF-10FF6CFE8B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Shopping Iguatemi Fortaleza</t>
   </si>
   <si>
-    <t>Shopping União de Osasco</t>
-  </si>
-  <si>
     <t>Shopping Center Interlagos</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Shopping Center Leste Aricanduva</t>
   </si>
   <si>
-    <t>Ribeirão Shopping</t>
-  </si>
-  <si>
     <t>Shopping Morumbi</t>
   </si>
   <si>
@@ -90,12 +84,6 @@
     <t>Palladium Shopping Curitiba</t>
   </si>
   <si>
-    <t>Passei das Águas Shopping</t>
-  </si>
-  <si>
-    <t>Center Shopping Uberlândia</t>
-  </si>
-  <si>
     <t>Shopping Recife</t>
   </si>
   <si>
@@ -111,9 +99,6 @@
     <t>Shopping Ibirapuera</t>
   </si>
   <si>
-    <t>Novo Shopping Ribeirão Preto</t>
-  </si>
-  <si>
     <t>Iguatemi Campinas</t>
   </si>
   <si>
@@ -274,6 +259,21 @@
   </si>
   <si>
     <t>pythonimpressionador+maria_luiza@gmail.com</t>
+  </si>
+  <si>
+    <t>Shopping Uniao de Osasco</t>
+  </si>
+  <si>
+    <t>Passei das Aguas Shopping</t>
+  </si>
+  <si>
+    <t>Ribeirao Shopping</t>
+  </si>
+  <si>
+    <t>Center Shopping Uberlandia</t>
+  </si>
+  <si>
+    <t>Novo Shopping Ribeirao Preto</t>
   </si>
 </sst>
 </file>
@@ -636,19 +636,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D81E77-7AEF-4DB7-8688-DEDDD091CFFB}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,322 +659,378 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{71E13B65-9239-473E-B00B-24152BE46E62}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E3106FEB-106F-4653-B503-E2D2031143F8}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{B6EBA633-9A57-4B4B-96B4-C65CFAD1BB3E}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{7823E53E-AF09-484D-A82D-90E56D3B173C}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{3741F77C-FA16-4C22-B015-4FDF829B5647}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{E0868D17-25A2-487B-AA15-484F6B02EBA7}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{B6F8659F-A0CB-412D-AE6A-9DA852BFAA32}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{4CFCBEB2-A644-4E59-9788-1DDF09FAF464}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{38F81A3D-BB76-4DBF-B55C-183FC4B858A7}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{98973E91-31EC-40FD-86B0-ED8A4168C6E8}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{03A322C5-0A08-4680-8550-E77955A4AE16}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{E5CB0419-824E-4DB2-A37A-D3C4C77E1115}"/>
-    <hyperlink ref="C15" r:id="rId13" xr:uid="{59E0BF81-A494-4E83-8798-A91BEBA8D604}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{ACE724F6-B50F-4C54-BEB0-05F796CEB518}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{97ADDF58-A02A-4AB6-92C6-A696B385AA7C}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{468AA824-B854-4C50-AE64-62AB564D2BC8}"/>
-    <hyperlink ref="C19" r:id="rId17" xr:uid="{D68730A0-9B08-47EA-B08B-D9AF34A604C6}"/>
-    <hyperlink ref="C20" r:id="rId18" xr:uid="{DC9B9350-B3A1-42F7-AC7F-FA19215DAC1C}"/>
-    <hyperlink ref="C21" r:id="rId19" xr:uid="{2B72A44B-E3AB-4DC9-843D-E086A5935BBD}"/>
-    <hyperlink ref="C22" r:id="rId20" xr:uid="{86DE27C8-7A8B-4539-BDDF-78A25128E590}"/>
-    <hyperlink ref="C23" r:id="rId21" xr:uid="{DA1C7256-28A5-4CC6-B93E-1D00A4600C54}"/>
-    <hyperlink ref="C24" r:id="rId22" xr:uid="{4218CF6B-06BF-4E28-B5ED-DB65662FB86F}"/>
-    <hyperlink ref="C25" r:id="rId23" xr:uid="{AFD4FC21-C827-47BB-A10B-8F182A528B87}"/>
-    <hyperlink ref="C26" r:id="rId24" xr:uid="{A077F048-53D0-4C90-9D38-4531C608CEEB}"/>
-    <hyperlink ref="C27" r:id="rId25" xr:uid="{9146DF61-FD66-4AC6-8767-2D00EC98E736}"/>
-    <hyperlink ref="C14" r:id="rId26" xr:uid="{5FFD0C79-EDBB-417E-98DA-5E77D27BBC40}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{254AFD77-5655-433E-A791-AC365E3B42FC}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{D635E467-F7EB-489C-9D95-7BB949741457}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{94E49A35-7A1E-442C-9F81-1B85E47C65DE}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{D1DD7001-848D-44F1-9BE5-43A1E14CEDAE}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{E957A8E6-0313-478C-94B4-B7FF03DF4DBA}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{24292EA9-A868-44CF-972D-FE3381285C7C}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{BCF095C0-73C3-4B2B-91F3-350135CA6F8D}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{8F88853D-1E1F-427C-BF29-598913F57AE6}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{9FBB1C19-F965-4A4F-8C1F-52E084D3E305}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{8ACCC45A-48A0-4979-99B9-22C92438F0CD}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{8029907C-F1EE-4BF8-A616-1A1204A7938F}"/>
+    <hyperlink ref="C15" r:id="rId12" xr:uid="{0C59AD50-1128-4ACA-9B3D-36FED7B624B6}"/>
+    <hyperlink ref="C16" r:id="rId13" xr:uid="{8DA90E6F-2972-4843-9138-B93401B705EC}"/>
+    <hyperlink ref="C17" r:id="rId14" xr:uid="{4E4090C4-14D2-46F2-8923-03E5855254E3}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{F5CDAF44-E913-4E8A-ACE6-F3C655BD2F3E}"/>
+    <hyperlink ref="C19" r:id="rId16" xr:uid="{3FAC4272-4F77-4DB3-9328-0187DA78ACDE}"/>
+    <hyperlink ref="C20" r:id="rId17" xr:uid="{41755118-D2D2-4B5E-9678-7225156333D7}"/>
+    <hyperlink ref="C21" r:id="rId18" xr:uid="{EF68A700-B1D0-42C1-88EC-89CEF6654D05}"/>
+    <hyperlink ref="C22" r:id="rId19" xr:uid="{C2D07C02-75DE-4A2C-82B0-CB0F78C873D9}"/>
+    <hyperlink ref="C23" r:id="rId20" xr:uid="{75128265-5B33-4F11-888D-953D0EC1E8EB}"/>
+    <hyperlink ref="C24" r:id="rId21" xr:uid="{D768EFD2-C51E-4CB1-9931-5F85FE793235}"/>
+    <hyperlink ref="C25" r:id="rId22" xr:uid="{BEF41F7F-6444-4ED3-B8BE-1BE73B69107C}"/>
+    <hyperlink ref="C26" r:id="rId23" xr:uid="{F953CA09-3009-4BA6-821A-AFBC2FEAF82B}"/>
+    <hyperlink ref="C27" r:id="rId24" xr:uid="{3E9434B3-D190-4C12-B2E1-FC864CEBC2C6}"/>
+    <hyperlink ref="C14" r:id="rId25" xr:uid="{9BAB4C2A-D231-4166-9E62-DEC7245CAB93}"/>
+    <hyperlink ref="C6" r:id="rId26" xr:uid="{F96AC10D-6C62-47AE-B14B-FBFF7532E73B}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>